<commit_message>
Preliminary check-in: Update to some ODK Survey forms to rename them to the table_id so that we generate definitions.csv and properties.csv ; update to process a properties sheet into the properties.csv ; minimize the content of the properties.csv
</commit_message>
<xml_diff>
--- a/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
+++ b/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\adult_coverage\forms\adult_coverage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="2420" windowWidth="30140" windowHeight="21620" tabRatio="282" activeTab="3"/>
+    <workbookView xWindow="7645" yWindow="2422" windowWidth="30135" windowHeight="21626" tabRatio="282" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -165,9 +170,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>form_id</t>
-  </si>
-  <si>
     <t>form_version</t>
   </si>
   <si>
@@ -643,6 +645,9 @@
   </si>
   <si>
     <t>disableSwipeNavigation</t>
+  </si>
+  <si>
+    <t>table_id</t>
   </si>
 </sst>
 </file>
@@ -787,6 +792,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1085,7 +1093,7 @@
       <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
@@ -1096,57 +1104,57 @@
     <col min="9" max="9" width="35.5" customWidth="1"/>
     <col min="10" max="10" width="41" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="12" max="12" width="26.375" customWidth="1"/>
     <col min="13" max="13" width="20.5" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.875" customWidth="1"/>
     <col min="16" max="17" width="18.5" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15.125" customWidth="1"/>
     <col min="23" max="23" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>3</v>
@@ -1170,24 +1178,24 @@
         <v>9</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1206,7 +1214,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -1217,10 +1225,10 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -1235,7 +1243,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1243,11 +1251,11 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="8"/>
@@ -1263,10 +1271,10 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1274,13 +1282,13 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="8"/>
@@ -1296,10 +1304,10 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1307,11 +1315,11 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="8"/>
@@ -1327,10 +1335,10 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1338,13 +1346,13 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="8"/>
@@ -1360,10 +1368,10 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1375,10 +1383,10 @@
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -1393,10 +1401,10 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1404,11 +1412,11 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="8"/>
@@ -1424,10 +1432,10 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1435,13 +1443,13 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="8"/>
@@ -1457,10 +1465,10 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1468,11 +1476,11 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="8"/>
@@ -1488,10 +1496,10 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1499,13 +1507,13 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="8"/>
@@ -1521,10 +1529,10 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1536,10 +1544,10 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -1554,10 +1562,10 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1569,10 +1577,10 @@
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1587,10 +1595,10 @@
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17.5" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1598,11 +1606,11 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="8"/>
@@ -1618,10 +1626,10 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
       <c r="W15" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1629,13 +1637,13 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="8"/>
@@ -1651,268 +1659,268 @@
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
       <c r="W16" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="7:23" ht="17.5" customHeight="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G17" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" s="12"/>
       <c r="W17" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="12"/>
       <c r="W18" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="7:23" ht="17.5" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="W19" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G20" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J20" s="12"/>
       <c r="W20" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G21" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J21" s="12"/>
       <c r="W21" s="16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="7:23" ht="17.5" customHeight="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G22" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J22" s="12"/>
       <c r="W22" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G23" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J23" s="12"/>
       <c r="W23" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="7:23" ht="17.5" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G24" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="W24" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="7:23" ht="17.5" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G25" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="W25" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="7:23" ht="17.5" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G26" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J26" s="12"/>
       <c r="W26" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G27" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J27" s="12"/>
       <c r="W27" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G28" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="W28" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="7:23" ht="17.5" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G29" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J29" s="12"/>
       <c r="W29" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G30" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J30" s="12"/>
       <c r="W30" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="7:23" ht="17.5" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G31" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="W31" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="7:23" ht="17.5" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="W32" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="3:23" ht="17.5" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J33" s="12"/>
       <c r="W33" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G34" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J34" s="12"/>
       <c r="W34" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1922,52 +1930,52 @@
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="W35" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J36" s="12"/>
       <c r="W36" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J37" s="12"/>
       <c r="W37" s="16" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1976,529 +1984,529 @@
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W38" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>13</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W39" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W40" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W41" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="3:23" ht="17.5" customHeight="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G42" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W42" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G43" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W43" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W44" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G45" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W45" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W46" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G47" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="W47" s="14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="3:23" ht="17.5" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G48" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="W48" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="7:23" ht="17.5" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G49" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W49" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G50" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W50" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="7:23" ht="17.5" customHeight="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G51" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W51" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="7:23" ht="17.5" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G52" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W52" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G53" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W53" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="7:23" ht="17.5" customHeight="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G54" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="W54" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="7:23" ht="17.5" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G55" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="W55" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G56" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W56" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G57" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W57" s="16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="7:23" ht="17.5" customHeight="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G58" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W58" s="14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G59" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W59" s="16" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" spans="7:23" ht="17.5" customHeight="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G60" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W60" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G61" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W61" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G62" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W62" s="16" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="7:23" ht="17.5" customHeight="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G63" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H63" s="8"/>
       <c r="I63" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W63" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G64" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I64" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W64" s="16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="3:23" ht="17.5" customHeight="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G65" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H65" s="8"/>
       <c r="I65" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W65" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="3:23" ht="17.5" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G66" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H66" s="11"/>
       <c r="I66" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="W66" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="3:23" ht="17.5" customHeight="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
         <v>13</v>
       </c>
       <c r="I67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W67" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="3:23" ht="17.5" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
         <v>13</v>
       </c>
       <c r="I68" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W68" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="3:23" ht="17.5" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
         <v>13</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="W69" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="70" spans="3:23" ht="17.5" customHeight="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
         <v>13</v>
       </c>
       <c r="I70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W70" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="3:23" ht="17.5" customHeight="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
         <v>13</v>
       </c>
       <c r="I71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J71" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="W71" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" spans="3:23" ht="17.5" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G72" t="s">
         <v>13</v>
       </c>
       <c r="I72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J72" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="W72" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="3:23" ht="17.5" customHeight="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G73" t="s">
         <v>13</v>
       </c>
       <c r="I73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="W73" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="74" spans="3:23" ht="17.5" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="76" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="77" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="78" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="79" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="80" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="81" ht="17.5" customHeight="1"/>
-    <row r="82" ht="17.5" customHeight="1"/>
-    <row r="83" ht="17.5" customHeight="1"/>
-    <row r="84" ht="17.5" customHeight="1"/>
-    <row r="85" ht="17.5" customHeight="1"/>
-    <row r="86" ht="17.5" customHeight="1"/>
-    <row r="87" ht="17.5" customHeight="1"/>
-    <row r="88" ht="17.5" customHeight="1"/>
-    <row r="89" ht="17.5" customHeight="1"/>
-    <row r="90" ht="17.5" customHeight="1"/>
-    <row r="91" ht="17.5" customHeight="1"/>
-    <row r="92" ht="17.5" customHeight="1"/>
-    <row r="93" ht="17.5" customHeight="1"/>
-    <row r="94" ht="17.5" customHeight="1"/>
-    <row r="95" ht="17.5" customHeight="1"/>
-    <row r="96" ht="17.5" customHeight="1"/>
-    <row r="97" ht="17.5" customHeight="1"/>
-    <row r="98" ht="17.5" customHeight="1"/>
-    <row r="99" ht="17.5" customHeight="1"/>
-    <row r="100" ht="17.5" customHeight="1"/>
-    <row r="101" ht="17.5" customHeight="1"/>
-    <row r="102" ht="17.5" customHeight="1"/>
-    <row r="103" ht="17.5" customHeight="1"/>
-    <row r="104" ht="17.5" customHeight="1"/>
+    <row r="75" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2518,242 +2526,242 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="147.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.125" customWidth="1"/>
+    <col min="2" max="2" width="147.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="11" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="14" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="15" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="17" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="18" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A17" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="7" t="s">
+    <row r="20" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="21" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="24" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2774,25 +2782,25 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -2803,7 +2811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2825,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2836,7 +2844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2847,7 +2855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2858,7 +2866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2869,7 +2877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2880,7 +2888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2891,8 +2899,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2903,7 +2911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2914,7 +2922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2925,7 +2933,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2936,7 +2944,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2947,7 +2955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2969,7 +2977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -2980,7 +2988,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2991,7 +2999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -3002,8 +3010,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3014,7 +3022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -3025,49 +3033,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="11" t="s">
+    <row r="28" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1">
+    </row>
+    <row r="30" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="C30" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3085,61 +3093,61 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
+    <col min="3" max="3" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="B3" s="1">
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Revert "Merge pull request #37 from clarlars/clarlars-customFormFix"
This reverts commit 21108979ce6e37cd5d380dab6cdb9c6ac0ed17f7, reversing
changes made to cacecb63cabc294f58c86999d7ca882d7da6464f.
</commit_message>
<xml_diff>
--- a/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
+++ b/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\adult_coverage\forms\adult_coverage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20320" yWindow="3820" windowWidth="30140" windowHeight="21620" tabRatio="282"/>
+    <workbookView xWindow="7645" yWindow="2422" windowWidth="30135" windowHeight="21626" tabRatio="282" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -618,6 +623,9 @@
     <t>screen.templatePath</t>
   </si>
   <si>
+    <t>../tables/adult_coverage/forms/adult_coverage/VR_adult_coverage.handlebars</t>
+  </si>
+  <si>
     <t>disableSwipeNavigation</t>
   </si>
   <si>
@@ -640,15 +648,12 @@
   </si>
   <si>
     <t>display.title.text</t>
-  </si>
-  <si>
-    <t>../config/tables/adult_coverage/forms/adult_coverage/VR_adult_coverage.handlebars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -838,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -890,7 +895,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1118,35 +1123,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="9" max="9" width="35.5" customWidth="1"/>
     <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.875" customWidth="1"/>
+    <col min="12" max="12" width="26.375" customWidth="1"/>
     <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="21.1640625" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="21.125" customWidth="1"/>
+    <col min="15" max="15" width="15.875" customWidth="1"/>
     <col min="16" max="17" width="18.5" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="20" max="20" width="29.83203125" customWidth="1"/>
+    <col min="20" max="20" width="29.875" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15.125" customWidth="1"/>
     <col min="23" max="23" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>53</v>
@@ -1173,19 +1177,19 @@
         <v>2</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>3</v>
@@ -1203,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>8</v>
@@ -1212,10 +1216,10 @@
         <v>56</v>
       </c>
       <c r="W1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
@@ -1226,7 +1230,7 @@
         <v>196</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1245,7 +1249,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -1274,7 +1278,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1305,7 +1309,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1338,7 +1342,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1369,7 +1373,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1402,7 +1406,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+    <row r="8" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1435,7 +1439,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+    <row r="9" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1466,7 +1470,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1499,7 +1503,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+    <row r="11" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1530,7 +1534,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1563,7 +1567,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+    <row r="13" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1596,7 +1600,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+    <row r="14" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1629,7 +1633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="17.5" customHeight="1">
+    <row r="15" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1660,7 +1664,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1693,7 +1697,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="7:23" ht="17.5" customHeight="1">
+    <row r="17" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G17" s="14" t="s">
         <v>65</v>
       </c>
@@ -1706,7 +1710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16" t="s">
         <v>144</v>
       </c>
@@ -1721,7 +1725,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="7:23" ht="17.5" customHeight="1">
+    <row r="19" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="17" t="s">
         <v>12</v>
       </c>
@@ -1736,7 +1740,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G20" s="14" t="s">
         <v>65</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G21" s="16" t="s">
         <v>144</v>
       </c>
@@ -1764,7 +1768,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="7:23" ht="17.5" customHeight="1">
+    <row r="22" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G22" s="14" t="s">
         <v>65</v>
       </c>
@@ -1777,7 +1781,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G23" s="16" t="s">
         <v>144</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="7:23" ht="17.5" customHeight="1">
+    <row r="24" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G24" s="17" t="s">
         <v>12</v>
       </c>
@@ -1807,7 +1811,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="7:23" ht="17.5" customHeight="1">
+    <row r="25" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G25" s="17" t="s">
         <v>12</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="7:23" ht="17.5" customHeight="1">
+    <row r="26" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G26" s="14" t="s">
         <v>65</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G27" s="16" t="s">
         <v>144</v>
       </c>
@@ -1850,7 +1854,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G28" s="17" t="s">
         <v>12</v>
       </c>
@@ -1865,7 +1869,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="7:23" ht="17.5" customHeight="1">
+    <row r="29" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G29" s="14" t="s">
         <v>65</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G30" s="16" t="s">
         <v>144</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="7:23" ht="17.5" customHeight="1">
+    <row r="31" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G31" s="17" t="s">
         <v>12</v>
       </c>
@@ -1908,7 +1912,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="7:23" ht="17.5" customHeight="1">
+    <row r="32" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="17" t="s">
         <v>12</v>
       </c>
@@ -1923,7 +1927,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="3:23" ht="17.5" customHeight="1">
+    <row r="33" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="14" t="s">
         <v>65</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G34" s="16" t="s">
         <v>144</v>
       </c>
@@ -1951,7 +1955,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1970,7 +1974,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+    <row r="36" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1987,7 +1991,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -2006,7 +2010,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1">
+    <row r="38" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -2024,7 +2028,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1">
+    <row r="39" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="11" t="s">
         <v>65</v>
       </c>
@@ -2049,7 +2053,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="6" t="s">
         <v>144</v>
       </c>
@@ -2063,7 +2067,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="3:23" ht="17.5" customHeight="1">
+    <row r="42" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G42" s="14" t="s">
         <v>65</v>
       </c>
@@ -2075,7 +2079,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G43" s="16" t="s">
         <v>144</v>
       </c>
@@ -2089,7 +2093,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1">
+    <row r="44" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="17" t="s">
         <v>12</v>
       </c>
@@ -2104,7 +2108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1">
+    <row r="45" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G45" s="14" t="s">
         <v>65</v>
       </c>
@@ -2116,7 +2120,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="16" t="s">
         <v>144</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1">
+    <row r="47" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G47" s="17" t="s">
         <v>12</v>
       </c>
@@ -2145,7 +2149,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="3:23" ht="17.5" customHeight="1">
+    <row r="48" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G48" s="11" t="s">
         <v>12</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="7:23" ht="17.5" customHeight="1">
+    <row r="49" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G49" s="14" t="s">
         <v>65</v>
       </c>
@@ -2172,7 +2176,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G50" s="16" t="s">
         <v>144</v>
       </c>
@@ -2186,7 +2190,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="7:23" ht="17.5" customHeight="1">
+    <row r="51" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G51" s="17" t="s">
         <v>12</v>
       </c>
@@ -2201,7 +2205,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="7:23" ht="17.5" customHeight="1">
+    <row r="52" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G52" s="14" t="s">
         <v>65</v>
       </c>
@@ -2213,7 +2217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G53" s="16" t="s">
         <v>144</v>
       </c>
@@ -2227,7 +2231,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="54" spans="7:23" ht="17.5" customHeight="1">
+    <row r="54" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G54" s="17" t="s">
         <v>12</v>
       </c>
@@ -2242,7 +2246,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="7:23" ht="17.5" customHeight="1">
+    <row r="55" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G55" s="11" t="s">
         <v>12</v>
       </c>
@@ -2257,7 +2261,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G56" s="11" t="s">
         <v>65</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G57" s="6" t="s">
         <v>144</v>
       </c>
@@ -2282,7 +2286,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="7:23" ht="17.5" customHeight="1">
+    <row r="58" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G58" s="14" t="s">
         <v>65</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G59" s="16" t="s">
         <v>144</v>
       </c>
@@ -2308,7 +2312,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="7:23" ht="17.5" customHeight="1">
+    <row r="60" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G60" s="17" t="s">
         <v>12</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G61" s="14" t="s">
         <v>65</v>
       </c>
@@ -2335,7 +2339,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G62" s="16" t="s">
         <v>144</v>
       </c>
@@ -2349,7 +2353,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="7:23" ht="17.5" customHeight="1">
+    <row r="63" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G63" s="14" t="s">
         <v>65</v>
       </c>
@@ -2361,7 +2365,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G64" s="16" t="s">
         <v>144</v>
       </c>
@@ -2375,7 +2379,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="3:23" ht="17.5" customHeight="1">
+    <row r="65" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G65" s="17" t="s">
         <v>12</v>
       </c>
@@ -2390,7 +2394,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="3:23" ht="17.5" customHeight="1">
+    <row r="66" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G66" s="11" t="s">
         <v>12</v>
       </c>
@@ -2405,7 +2409,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="3:23" ht="17.5" customHeight="1">
+    <row r="67" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
         <v>12</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="3:23" ht="17.5" customHeight="1">
+    <row r="68" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
         <v>12</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="3:23" ht="17.5" customHeight="1">
+    <row r="69" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
         <v>12</v>
       </c>
@@ -2447,7 +2451,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="3:23" ht="17.5" customHeight="1">
+    <row r="70" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
         <v>12</v>
       </c>
@@ -2461,7 +2465,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="3:23" ht="17.5" customHeight="1">
+    <row r="71" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
         <v>12</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="3:23" ht="17.5" customHeight="1">
+    <row r="72" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G72" t="s">
         <v>12</v>
       </c>
@@ -2489,7 +2493,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="3:23" ht="17.5" customHeight="1">
+    <row r="73" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G73" t="s">
         <v>12</v>
       </c>
@@ -2503,41 +2507,41 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="3:23" ht="17.5" customHeight="1">
+    <row r="74" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="76" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="77" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="78" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="79" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="80" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="81" ht="17.5" customHeight="1"/>
-    <row r="82" ht="17.5" customHeight="1"/>
-    <row r="83" ht="17.5" customHeight="1"/>
-    <row r="84" ht="17.5" customHeight="1"/>
-    <row r="85" ht="17.5" customHeight="1"/>
-    <row r="86" ht="17.5" customHeight="1"/>
-    <row r="87" ht="17.5" customHeight="1"/>
-    <row r="88" ht="17.5" customHeight="1"/>
-    <row r="89" ht="17.5" customHeight="1"/>
-    <row r="90" ht="17.5" customHeight="1"/>
-    <row r="91" ht="17.5" customHeight="1"/>
-    <row r="92" ht="17.5" customHeight="1"/>
-    <row r="93" ht="17.5" customHeight="1"/>
-    <row r="94" ht="17.5" customHeight="1"/>
-    <row r="95" ht="17.5" customHeight="1"/>
-    <row r="96" ht="17.5" customHeight="1"/>
-    <row r="97" ht="17.5" customHeight="1"/>
-    <row r="98" ht="17.5" customHeight="1"/>
-    <row r="99" ht="17.5" customHeight="1"/>
-    <row r="100" ht="17.5" customHeight="1"/>
-    <row r="101" ht="17.5" customHeight="1"/>
-    <row r="102" ht="17.5" customHeight="1"/>
-    <row r="103" ht="17.5" customHeight="1"/>
-    <row r="104" ht="17.5" customHeight="1"/>
+    <row r="75" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2557,13 +2561,13 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="147.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.125" customWidth="1"/>
+    <col min="2" max="2" width="147.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>66</v>
       </c>
@@ -2579,7 +2583,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+    <row r="3" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
+    <row r="4" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -2595,7 +2599,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1">
+    <row r="5" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" customHeight="1">
+    <row r="6" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" customHeight="1">
+    <row r="7" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2619,7 +2623,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75" customHeight="1">
+    <row r="8" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2627,7 +2631,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.75" customHeight="1">
+    <row r="9" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.75" customHeight="1">
+    <row r="10" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -2643,7 +2647,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.75" customHeight="1">
+    <row r="11" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.75" customHeight="1">
+    <row r="12" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>88</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
+    <row r="13" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2667,7 +2671,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
+    <row r="14" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
+    <row r="15" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -2683,7 +2687,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.75" customHeight="1">
+    <row r="16" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -2691,7 +2695,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" customHeight="1">
+    <row r="17" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>96</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="12.75" customHeight="1">
+    <row r="18" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>98</v>
       </c>
@@ -2707,7 +2711,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.75" customHeight="1">
+    <row r="19" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2715,7 +2719,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.75" customHeight="1">
+    <row r="20" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>101</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="12.75" customHeight="1">
+    <row r="21" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>103</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.75" customHeight="1">
+    <row r="22" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -2739,7 +2743,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.75" customHeight="1">
+    <row r="23" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2747,7 +2751,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.75" customHeight="1">
+    <row r="24" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2755,7 +2759,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="12.75" customHeight="1">
+    <row r="25" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>109</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.75" customHeight="1">
+    <row r="26" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>110</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="12.75" customHeight="1">
+    <row r="27" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -2779,7 +2783,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.75" customHeight="1">
+    <row r="28" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="12.75" customHeight="1">
+    <row r="29" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2809,18 +2813,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -2828,10 +2832,10 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2842,7 +2846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2908,7 +2912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2919,7 +2923,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2930,8 +2934,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2942,7 +2946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2953,7 +2957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2964,7 +2968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2975,7 +2979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2986,7 +2990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3008,7 +3012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3019,7 +3023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3030,7 +3034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3041,8 +3045,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -3053,7 +3057,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3064,8 +3068,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>59</v>
       </c>
@@ -3076,7 +3080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
+    <row r="27" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>59</v>
       </c>
@@ -3087,7 +3091,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
+    <row r="28" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>59</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1">
+    <row r="30" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>142</v>
       </c>
@@ -3127,14 +3131,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
+    <col min="3" max="3" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -3142,18 +3146,18 @@
         <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
+    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -3161,7 +3165,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
@@ -3169,16 +3173,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1">
+    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>